<commit_message>
2. normálforma, still ugly
</commit_message>
<xml_diff>
--- a/2018-09-14_Minta.xlsx
+++ b/2018-09-14_Minta.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jaksics_Benedek\Adatbázis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Normalizalas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="1.normálforma" sheetId="1" r:id="rId1"/>
+    <sheet name="2.normálforma" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
   <si>
     <t>Rendszám</t>
   </si>
@@ -420,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" activeCellId="2" sqref="A1:A1048576 G1:G1048576 J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,4 +611,181 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
+        <v>43357</v>
+      </c>
+      <c r="F2" s="1">
+        <v>43365</v>
+      </c>
+      <c r="G2">
+        <v>550</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43357</v>
+      </c>
+      <c r="F3" s="1">
+        <v>43365</v>
+      </c>
+      <c r="G3">
+        <v>1375</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>